<commit_message>
fix bug for csv file name conflict
</commit_message>
<xml_diff>
--- a/data/excel/final_excel.xlsx
+++ b/data/excel/final_excel.xlsx
@@ -400,7 +400,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2020年2月10日云闪付APP总体交易商户24.39万, 环比下降1.44%, 同比增长36.96%。当日新增交易商户0.0家, 环比下降-33.33%, 同比增长14.29%。新增商户主要集中在辽宁、湖北、重庆等地区。二维码交易商户23.94万, 占总交易商户的98.17%, 环比下降1.48%;手机支付控件交易商户3104.0家, 占总交易商户的1.27%, 环比下降-0.74%;手机外部支付交易商户2257.0家, 环比下降-0.79%;</t>
+          <t>2020年2月13日云闪付APP总体交易商户24.32万, 环比增长-1.25%, 同比增长10.45%。当日新增交易商户29.0家, 环比增长-14.71%, 同比增长-97.07%。新增商户主要集中在辽宁、湖北、重庆等地区。二维码交易商户23.84万, 占总交易商户的98.01%, 环比增长-1.3%；手机支付控件交易商户3508.0家, 占总交易商户的1.44%, 环比增长2.07%；手机外部支付交易商户2607.0家, 环比增长2.92%；</t>
         </is>
       </c>
     </row>
@@ -436,7 +436,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3、交易金额整体偏低，交易金额在10元以下的占比达56.74%。</t>
+          <t>3、交易金额整体偏低，交易金额在10元以下的占比达61.60%。</t>
         </is>
       </c>
     </row>
@@ -501,21 +501,21 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1084133</v>
+        <v>1270928</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>56.74%</t>
+          <t>61.60%</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-0.01931282525375788</v>
+        <v>-0.01384191246361832</v>
       </c>
       <c r="F2" t="n">
-        <v>54725</v>
+        <v>58914</v>
       </c>
       <c r="G2" t="n">
-        <v>19.81056190041115</v>
+        <v>21.57259734528295</v>
       </c>
     </row>
     <row r="3">
@@ -528,21 +528,21 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>390316</v>
+        <v>378173</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20.43%</t>
+          <t>18.33%</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>-0.1963151023971601</v>
+        <v>-0.1785758503172331</v>
       </c>
       <c r="F3" t="n">
-        <v>58285</v>
+        <v>60355</v>
       </c>
       <c r="G3" t="n">
-        <v>6.696680106373853</v>
+        <v>6.265810620495402</v>
       </c>
     </row>
     <row r="4">
@@ -555,21 +555,21 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>85412</v>
+        <v>83600</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.47%</t>
+          <t>4.05%</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>-0.1169239358567425</v>
+        <v>0.01222908342414341</v>
       </c>
       <c r="F4" t="n">
-        <v>23042</v>
+        <v>22942</v>
       </c>
       <c r="G4" t="n">
-        <v>3.706796285044701</v>
+        <v>3.643971754860082</v>
       </c>
     </row>
     <row r="5">
@@ -582,21 +582,21 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>327134</v>
+        <v>307783</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17.12%</t>
+          <t>14.92%</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-0.009279280916298704</v>
+        <v>-0.001450215747980433</v>
       </c>
       <c r="F5" t="n">
-        <v>140392</v>
+        <v>134730</v>
       </c>
       <c r="G5" t="n">
-        <v>2.330147016924041</v>
+        <v>2.284442959994062</v>
       </c>
     </row>
     <row r="6">
@@ -609,21 +609,21 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>23851</v>
+        <v>22663</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.25%</t>
+          <t>1.10%</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.08744813750968849</v>
+        <v>0.004699206454759075</v>
       </c>
       <c r="F6" t="n">
-        <v>12304</v>
+        <v>10827</v>
       </c>
       <c r="G6" t="n">
-        <v>1.938475292587776</v>
+        <v>2.093192943567008</v>
       </c>
     </row>
   </sheetData>
@@ -658,7 +658,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>当日，手机支付控件交易130.06万笔，环比下降-1.88%，同比下降-21.16%。其中手机外部支付控件交易24.25万笔，环比增长-4.88%，同比下降-81.39%，占总控件交易笔数的18.64%。</t>
+          <t>当日，手机支付控件交易122.8万笔，环比增长-2.47%，同比增长-29.88%。其中手机外部支付控件交易23.43万笔，环比增长-2.62%，同比增长-82.42%，占总控件交易笔数的19.08%。</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1、手机支付控件TOP10商户主要是信用卡还款业务、以内部商户为主，商户优惠交易占比仅为22.81%。</t>
+          <t>1、手机支付控件TOP10商户主要是信用卡还款业务、以内部商户为主，商户优惠交易占比仅为24.07%。</t>
         </is>
       </c>
     </row>
@@ -765,26 +765,26 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>信用卡还款</t>
+          <t>转账或信用卡还款</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>422280</v>
+        <v>418975</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-1.16%</t>
+          <t>-2.87%</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>323229</v>
+        <v>322389</v>
       </c>
       <c r="G2" t="n">
-        <v>90103</v>
+        <v>92874</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>21.34%</t>
+          <t>22.17%</t>
         </is>
       </c>
     </row>
@@ -803,22 +803,22 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>82719</v>
+        <v>67358</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>17.82%</t>
+          <t>-10.03%</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>72054</v>
+        <v>58597</v>
       </c>
       <c r="G3" t="n">
-        <v>15352</v>
+        <v>12642</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>18.56%</t>
+          <t>18.77%</t>
         </is>
       </c>
     </row>
@@ -828,7 +828,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>平安信用卡中心还款业务(深圳)</t>
+          <t>民生银行</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -837,22 +837,22 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>67871</v>
+        <v>57515</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-27.56%</t>
+          <t>-2.14%</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>61699</v>
+        <v>50874</v>
       </c>
       <c r="G4" t="n">
-        <v>11043</v>
+        <v>9125</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>16.27%</t>
+          <t>15.87%</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>光大卡中心信用卡还款（深圳线上）</t>
+          <t>平安信用卡中心还款业务(深圳)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -871,22 +871,22 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>57694</v>
+        <v>56990</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-11.57%</t>
+          <t>-5.78%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>49159</v>
+        <v>50866</v>
       </c>
       <c r="G5" t="n">
-        <v>8869</v>
+        <v>10086</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>15.37%</t>
+          <t>17.70%</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>民生银行</t>
+          <t>光大卡中心信用卡还款（深圳线上）</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -905,22 +905,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>54440</v>
+        <v>50950</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>7.80%</t>
+          <t>-0.91%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>47776</v>
+        <v>44211</v>
       </c>
       <c r="G6" t="n">
-        <v>8769</v>
+        <v>8297</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>16.11%</t>
+          <t>16.28%</t>
         </is>
       </c>
     </row>
@@ -930,31 +930,31 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>招行信用卡还款</t>
+          <t>U净</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>信用卡还款</t>
+          <t>外部商户</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>46971</v>
+        <v>48264</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12.23%</t>
+          <t>1.08%</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>42765</v>
+        <v>27840</v>
       </c>
       <c r="G7" t="n">
-        <v>7866</v>
+        <v>48228</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>16.75%</t>
+          <t>99.93%</t>
         </is>
       </c>
     </row>
@@ -964,31 +964,31 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>U净</t>
+          <t>广发信用卡还款(深圳)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>外部商户</t>
+          <t>信用卡还款</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>46598</v>
+        <v>43831</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-3.80%</t>
+          <t>0.23%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>27473</v>
+        <v>39104</v>
       </c>
       <c r="G8" t="n">
-        <v>45760</v>
+        <v>6812</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>98.20%</t>
+          <t>15.54%</t>
         </is>
       </c>
     </row>
@@ -998,7 +998,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>广发信用卡还款(深圳)</t>
+          <t>华夏银行信用卡中心</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1007,22 +1007,22 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>44303</v>
+        <v>40117</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>9.96%</t>
+          <t>43.94%</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>37196</v>
+        <v>34641</v>
       </c>
       <c r="G9" t="n">
-        <v>6882</v>
+        <v>6597</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>15.53%</t>
+          <t>16.44%</t>
         </is>
       </c>
     </row>
@@ -1041,22 +1041,22 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>42169</v>
+        <v>38112</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.62%</t>
+          <t>-8.89%</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>39315</v>
+        <v>34388</v>
       </c>
       <c r="G10" t="n">
-        <v>5503</v>
+        <v>5685</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>13.05%</t>
+          <t>14.92%</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>中信银行信用卡还款(深圳)</t>
+          <t>招行信用卡还款</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1075,22 +1075,22 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>33689</v>
+        <v>33934</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-31.67%</t>
+          <t>-2.79%</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>31354</v>
+        <v>31342</v>
       </c>
       <c r="G11" t="n">
-        <v>4876</v>
+        <v>5722</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>14.47%</t>
+          <t>16.86%</t>
         </is>
       </c>
     </row>
@@ -1187,22 +1187,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>46598</v>
+        <v>48264</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-3.80%</t>
+          <t>1.08%</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>27473</v>
+        <v>27840</v>
       </c>
       <c r="F2" t="n">
-        <v>45760</v>
+        <v>48228</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>98.20%</t>
+          <t>99.93%</t>
         </is>
       </c>
     </row>
@@ -1216,22 +1216,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>25424</v>
+        <v>27159</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.39%</t>
+          <t>1.00%</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>20133</v>
+        <v>22056</v>
       </c>
       <c r="F3" t="n">
-        <v>5732</v>
+        <v>6112</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>22.55%</t>
+          <t>22.50%</t>
         </is>
       </c>
     </row>
@@ -1241,26 +1241,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>浙江集享电子商务有限公司</t>
+          <t>上海甄会选电子商务有限公司</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>16735</v>
+        <v>13310</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>21.75%</t>
+          <t>3.09%</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>12128</v>
+        <v>6802</v>
       </c>
       <c r="F4" t="n">
-        <v>17417</v>
+        <v>13286</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>104.08%</t>
+          <t>99.82%</t>
         </is>
       </c>
     </row>
@@ -1270,26 +1270,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>上海甄会选电子商务有限公司</t>
+          <t>京东到家</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>12985</v>
+        <v>10168</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-1.84%</t>
+          <t>4.16%</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>6252</v>
+        <v>9065</v>
       </c>
       <c r="F5" t="n">
-        <v>13202</v>
+        <v>10147</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>101.67%</t>
+          <t>99.79%</t>
         </is>
       </c>
     </row>
@@ -1299,26 +1299,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>京东到家</t>
+          <t>浙江集享电子商务有限公司</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>11184</v>
+        <v>7295</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.04%</t>
+          <t>-38.73%</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>10050</v>
+        <v>5857</v>
       </c>
       <c r="F6" t="n">
-        <v>11234</v>
+        <v>7014</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>100.45%</t>
+          <t>96.15%</t>
         </is>
       </c>
     </row>
@@ -1332,22 +1332,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7063</v>
+        <v>6261</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-8.25%</t>
+          <t>0.55%</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6139</v>
+        <v>5698</v>
       </c>
       <c r="F7" t="n">
-        <v>6888</v>
+        <v>6036</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>97.52%</t>
+          <t>96.41%</t>
         </is>
       </c>
     </row>
@@ -1361,22 +1361,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4669</v>
+        <v>5315</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7.02%</t>
+          <t>6.07%</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>4142</v>
+        <v>4811</v>
       </c>
       <c r="F8" t="n">
-        <v>1288</v>
+        <v>1461</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>27.59%</t>
+          <t>27.49%</t>
         </is>
       </c>
     </row>
@@ -1390,22 +1390,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4463</v>
+        <v>3089</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>-22.98%</t>
+          <t>-3.38%</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3764</v>
+        <v>2637</v>
       </c>
       <c r="F9" t="n">
-        <v>1937</v>
+        <v>1314</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>43.40%</t>
+          <t>42.54%</t>
         </is>
       </c>
     </row>
@@ -1419,22 +1419,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2506</v>
+        <v>2347</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.47%</t>
+          <t>-2.49%</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F10" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1.68%</t>
+          <t>2.09%</t>
         </is>
       </c>
     </row>
@@ -1448,22 +1448,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2379</v>
+        <v>2247</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5.82%</t>
+          <t>-1.45%</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2037</v>
+        <v>1888</v>
       </c>
       <c r="F11" t="n">
-        <v>2448</v>
+        <v>2204</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>102.90%</t>
+          <t>98.09%</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2、当日，从商户入网分公司来看，上海、北京、黑龙江、青岛、广东、四川、厦门、浙江、云南、湖南地区交易量排名手机外部支付控件前十。</t>
+          <t>2、当日，从商户入网分公司来看，上海、北京、黑龙江、广东、厦门、四川、青岛、浙江、云南、江苏地区交易量排名手机外部支付控件前十。</t>
         </is>
       </c>
     </row>
@@ -1569,29 +1569,29 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>81601</v>
+        <v>83642</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>33.66%</t>
+          <t>35.70%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-9.17%</t>
+          <t>-1.39%</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>73279</v>
+        <v>72845</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>89.80%</t>
+          <t>87.09%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>-5.96%</t>
+          <t>-1.93%</t>
         </is>
       </c>
     </row>
@@ -1605,29 +1605,29 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>50331</v>
+        <v>50402</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20.76%</t>
+          <t>21.51%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-12.09%</t>
+          <t>-0.88%</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>27680</v>
+        <v>25806</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>55.00%</t>
+          <t>51.20%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>-11.98%</t>
+          <t>-2.54%</t>
         </is>
       </c>
     </row>
@@ -1641,29 +1641,29 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>25532</v>
+        <v>21200</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.53%</t>
+          <t>9.05%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-1.12%</t>
+          <t>-5.83%</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>668</v>
+        <v>547</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2.62%</t>
+          <t>2.58%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>-9.73%</t>
+          <t>-8.53%</t>
         </is>
       </c>
     </row>
@@ -1673,33 +1673,33 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>青岛</t>
+          <t>广东</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17385</v>
+        <v>11247</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7.17%</t>
+          <t>4.80%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20.24%</t>
+          <t>-3.63%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>17925</v>
+        <v>446</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>103.11%</t>
+          <t>3.97%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>20.06%</t>
+          <t>9.58%</t>
         </is>
       </c>
     </row>
@@ -1709,33 +1709,33 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>广东</t>
+          <t>厦门</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12717</v>
+        <v>10686</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5.25%</t>
+          <t>4.56%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-12.50%</t>
+          <t>4.01%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>395</v>
+        <v>2734</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3.11%</t>
+          <t>25.58%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>-20.20%</t>
+          <t>8.02%</t>
         </is>
       </c>
     </row>
@@ -1749,29 +1749,29 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10748</v>
+        <v>10193</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4.43%</t>
+          <t>4.35%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-1.98%</t>
+          <t>3.28%</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>251</v>
+        <v>343</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2.34%</t>
+          <t>3.37%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>-27.46%</t>
+          <t>37.20%</t>
         </is>
       </c>
     </row>
@@ -1781,33 +1781,33 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>厦门</t>
+          <t>青岛</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9072</v>
+        <v>7932</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3.74%</t>
+          <t>3.39%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>8.54%</t>
+          <t>-36.86%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2052</v>
+        <v>7326</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>22.62%</t>
+          <t>92.36%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>-12.61%</t>
+          <t>-37.71%</t>
         </is>
       </c>
     </row>
@@ -1821,29 +1821,29 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6910</v>
+        <v>6729</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.85%</t>
+          <t>2.87%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-16.98%</t>
+          <t>-12.74%</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2466</v>
+        <v>2463</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>35.69%</t>
+          <t>36.60%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>-32.86%</t>
+          <t>-17.27%</t>
         </is>
       </c>
     </row>
@@ -1857,29 +1857,29 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3760</v>
+        <v>3236</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.55%</t>
+          <t>1.38%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-12.94%</t>
+          <t>-7.12%</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2.63%</t>
+          <t>3.09%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>-6.60%</t>
+          <t>12.36%</t>
         </is>
       </c>
     </row>
@@ -1889,33 +1889,33 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3399</v>
+        <v>3230</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.40%</t>
+          <t>1.38%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>15.81%</t>
+          <t>-3.98%</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>686</v>
+        <v>1055</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>20.18%</t>
+          <t>32.66%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>-7.30%</t>
+          <t>-5.80%</t>
         </is>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3、当日，从交易用户归属地来看，广东、重庆、河北、云南、湖北、上海、河南、四川、湖南、深圳地区交易量排名手机外部支付控件前十。</t>
+          <t>3、当日，从交易用户归属地来看，广东、河北、重庆、云南、上海、河南、四川、深圳、湖北、江苏地区交易量排名手机外部支付控件前十。</t>
         </is>
       </c>
     </row>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>当日, 云闪付APP发生支付类交易448.96万笔其中远程转账、信用卡还款、被扫、一般主扫、快速收款码、小微主扫、外部控件、乘车码、人到人转账、公缴交易笔数排名前十，占到交易总量的98.93%。</t>
+          <t>当日, 云闪付APP发生支付类交易467.04万笔。其中远程转账、信用卡还款、被扫、一般主扫、快速收款码、小微主扫、手机外部支付控件、乘车码、人到人转账、公缴交易笔数排名前十，占到交易总量的98.65%。</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2057,107 +2057,107 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>24101</v>
+        <v>22952</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.55%</t>
+          <t>10.21%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-7.26%</t>
+          <t>-4.33%</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>15112</v>
+        <v>13950</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>62.70%</t>
+          <t>60.78%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>-8.62%</t>
+          <t>-7.25%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>重庆</t>
+          <t>河北</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17104</v>
+        <v>14924</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7.49%</t>
+          <t>6.64%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-4.07%</t>
+          <t>-0.92%</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3541</v>
+        <v>12528</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>20.70%</t>
+          <t>83.95%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>-6.79%</t>
+          <t>-1.99%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>河北</t>
+          <t>重庆</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>14992</v>
+        <v>14393</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6.56%</t>
+          <t>6.40%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2.30%</t>
+          <t>-5.11%</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>13025</v>
+        <v>3363</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>86.88%</t>
+          <t>23.37%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.88%</t>
+          <t>0.57%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -2165,65 +2165,65 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>13527</v>
+        <v>13575</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5.92%</t>
+          <t>6.04%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-0.72%</t>
+          <t>-1.40%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>10659</v>
+        <v>10193</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>78.80%</t>
+          <t>75.09%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2.04%</t>
+          <t>-1.73%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>湖北</t>
+          <t>上海</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>13361</v>
+        <v>12640</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5.85%</t>
+          <t>5.62%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-0.77%</t>
+          <t>-4.64%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2998</v>
+        <v>6809</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>22.44%</t>
+          <t>53.87%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>-10.53%</t>
+          <t>-8.74%</t>
         </is>
       </c>
     </row>
@@ -2233,177 +2233,177 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>上海</t>
+          <t>河南</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13187</v>
+        <v>12419</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5.77%</t>
+          <t>5.53%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-5.07%</t>
+          <t>3.15%</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>7684</v>
+        <v>9284</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>58.27%</t>
+          <t>74.76%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>-10.10%</t>
+          <t>4.43%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>河南</t>
+          <t>四川</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>12105</v>
+        <v>11402</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5.30%</t>
+          <t>5.07%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-3.77%</t>
+          <t>-4.77%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>9013</v>
+        <v>3009</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>74.46%</t>
+          <t>26.39%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>-10.32%</t>
+          <t>-8.60%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>四川</t>
+          <t>深圳</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>11950</v>
+        <v>10732</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5.23%</t>
+          <t>4.78%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-5.64%</t>
+          <t>-2.97%</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3471</v>
+        <v>7278</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>29.05%</t>
+          <t>67.82%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>3.09%</t>
+          <t>-5.17%</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>湖南</t>
+          <t>湖北</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>9146</v>
+        <v>10520</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.00%</t>
+          <t>4.68%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-0.97%</t>
+          <t>-10.09%</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3830</v>
+        <v>2722</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>41.88%</t>
+          <t>25.87%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>-9.22%</t>
+          <t>-16.32%</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>深圳</t>
+          <t>江苏</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9078</v>
+        <v>9315</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3.97%</t>
+          <t>4.15%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6.81%</t>
+          <t>-2.42%</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5469</v>
+        <v>5120</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>60.24%</t>
+          <t>54.97%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>-0.53%</t>
+          <t>-3.51%</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4、交易金额整体偏低。交易金额在10元以下的交易笔数占比达26.69%。</t>
+          <t>4、交易金额整体偏低。交易金额在10元以下的交易笔数占比达29.32%。</t>
         </is>
       </c>
     </row>
@@ -2504,23 +2504,23 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>64704</v>
+        <v>68686</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>26.69%</t>
+          <t>29.32%</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>466</v>
+        <v>551</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>20.65%</t>
+          <t>21.14%</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>138.8497854077253</v>
+        <v>124.6569872958258</v>
       </c>
     </row>
     <row r="3">
@@ -2533,23 +2533,23 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>61300</v>
+        <v>51421</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>25.28%</t>
+          <t>21.95%</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>828</v>
+        <v>1054</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>36.69%</t>
+          <t>40.43%</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>74.03381642512078</v>
+        <v>48.7865275142315</v>
       </c>
     </row>
     <row r="4">
@@ -2562,23 +2562,23 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>41999</v>
+        <v>37803</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17.32%</t>
+          <t>16.14%</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>837</v>
+        <v>963</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>37.08%</t>
+          <t>36.94%</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>50.17801672640383</v>
+        <v>39.25545171339564</v>
       </c>
     </row>
     <row r="5">
@@ -2591,23 +2591,23 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>67291</v>
+        <v>68568</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>27.75%</t>
+          <t>29.27%</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1241</v>
+        <v>1355</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>54.98%</t>
+          <t>51.98%</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>54.2232070910556</v>
+        <v>50.60369003690037</v>
       </c>
     </row>
     <row r="6">
@@ -2620,23 +2620,23 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7160</v>
+        <v>7797</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.95%</t>
+          <t>3.33%</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>618</v>
+        <v>628</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>27.38%</t>
+          <t>24.09%</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>11.58576051779935</v>
+        <v>12.4156050955414</v>
       </c>
     </row>
   </sheetData>
@@ -2690,13 +2690,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1137146</v>
+        <v>1204214</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2532873005089597</v>
+        <v>0.2578402479622678</v>
       </c>
       <c r="E2" t="n">
-        <v>0.006854942961066189</v>
+        <v>-0.021528241</v>
       </c>
     </row>
     <row r="3">
@@ -2709,13 +2709,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>965039</v>
+        <v>904582</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2149522780679578</v>
+        <v>0.1936845504056622</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.006481800820520212</v>
+        <v>-0.022950218</v>
       </c>
     </row>
     <row r="4">
@@ -2728,13 +2728,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>670286</v>
+        <v>703402</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1492991502489114</v>
+        <v>0.1506089001599011</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1583836308914691</v>
+        <v>-0.082281322</v>
       </c>
     </row>
     <row r="5">
@@ -2747,13 +2747,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>444996</v>
+        <v>472869</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09911817442728113</v>
+        <v>0.1012483331149361</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.04350274592410287</v>
+        <v>-0.039358609</v>
       </c>
     </row>
     <row r="6">
@@ -2766,13 +2766,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>424614</v>
+        <v>452245</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09457829849316747</v>
+        <v>0.09683242591407823</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02589291538716154</v>
+        <v>-0.030370275</v>
       </c>
     </row>
     <row r="7">
@@ -2785,13 +2785,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>272399</v>
+        <v>280366</v>
       </c>
       <c r="D7" t="n">
-        <v>0.06067400964461917</v>
+        <v>0.06003055848893069</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0107794607672156</v>
+        <v>-0.014319415</v>
       </c>
     </row>
     <row r="8">
@@ -2800,17 +2800,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>外部控件</t>
+          <t>手机外部支付控件</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>242454</v>
+        <v>234275</v>
       </c>
       <c r="D8" t="n">
-        <v>0.05400407613235179</v>
+        <v>0.05016178527351475</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.04877847830607289</v>
+        <v>-0.026199403</v>
       </c>
     </row>
     <row r="9">
@@ -2823,13 +2823,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>120767</v>
+        <v>183536</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02689957790869909</v>
+        <v>0.03929780566411185</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03309723006381632</v>
+        <v>0.011356936</v>
       </c>
     </row>
     <row r="10">
@@ -2842,13 +2842,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>96761</v>
+        <v>108580</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02155249412524641</v>
+        <v>0.02324860375626179</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0276995953395006</v>
+        <v>0.005947859000000001</v>
       </c>
     </row>
     <row r="11">
@@ -2861,13 +2861,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>67152</v>
+        <v>63171</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01495740107583165</v>
+        <v>0.01352585695235599</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.05387736699729486</v>
+        <v>-0.07310023</v>
       </c>
     </row>
     <row r="12">
@@ -2876,17 +2876,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>充值</t>
+          <t>无感支付</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>29055</v>
+        <v>29305</v>
       </c>
       <c r="D12" t="n">
-        <v>0.006471695381497032</v>
+        <v>0.006274639280505174</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.0311124449779912</v>
+        <v>-0.009631631999999999</v>
       </c>
     </row>
     <row r="13">
@@ -2895,17 +2895,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>无感支付</t>
+          <t>充值</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>13734</v>
+        <v>26692</v>
       </c>
       <c r="D13" t="n">
-        <v>0.003059103919101024</v>
+        <v>0.005715156856346839</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.006654129900188053</v>
+        <v>0.031574879</v>
       </c>
     </row>
     <row r="14">
@@ -2918,13 +2918,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4098</v>
+        <v>4308</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0009127863594346873</v>
+        <v>0.0009224073032047873</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.04852565590898537</v>
+        <v>-0.009882785999999999</v>
       </c>
     </row>
     <row r="15">
@@ -2937,13 +2937,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>830</v>
+        <v>2687</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0001848737624038044</v>
+        <v>0.0005753269321521039</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.5816532258064516</v>
+        <v>0.15669393</v>
       </c>
     </row>
     <row r="16">
@@ -2956,13 +2956,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>219</v>
+        <v>156</v>
       </c>
       <c r="D16" t="n">
-        <v>4.877994453787128e-05</v>
+        <v>3.340193577064689e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1648936170212766</v>
+        <v>0.06122449</v>
       </c>
     </row>
   </sheetData>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>当日, 二维码(含乘车码)交易笔数为191.08笔, 环比下降-6.33%, 同比增长-34.01%。其主要场景分布在零售、餐饮、其他场景, 占比分别达58.35%、13.61%、10.53%。</t>
+          <t>当日, 二维码(含乘车码)交易笔数为206.41笔, 环比增长-4.55%, 同比增长-52.23%。其主要场景分布在零售、公交地铁、餐饮场景, 占比分别达55.48%、13.41%、12.99%。</t>
         </is>
       </c>
     </row>
@@ -3067,29 +3067,29 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1114972</v>
+        <v>1144694</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>58.35%</t>
+          <t>55.48%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-8.50%</t>
+          <t>-4.84%</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>657016</v>
+        <v>685898</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-12.48%</t>
+          <t>-6.73%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>58.93%</t>
+          <t>59.92%</t>
         </is>
       </c>
     </row>
@@ -3099,33 +3099,33 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>餐饮</t>
+          <t>公交地铁</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>260032</v>
+        <v>276653</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13.61%</t>
+          <t>13.41%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-3.90%</t>
+          <t>1.29%</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>161922</v>
+        <v>260704</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-4.09%</t>
+          <t>1.22%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>62.27%</t>
+          <t>94.24%</t>
         </is>
       </c>
     </row>
@@ -3135,33 +3135,33 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>其他</t>
+          <t>餐饮</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>201219</v>
+        <v>267997</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.53%</t>
+          <t>12.99%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-6.64%</t>
+          <t>-5.66%</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>74162</v>
+        <v>168874</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-17.47%</t>
+          <t>-7.49%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>36.86%</t>
+          <t>63.01%</t>
         </is>
       </c>
     </row>
@@ -3171,33 +3171,33 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>公交地铁</t>
+          <t>其他</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>180363</v>
+        <v>215654</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9.44%</t>
+          <t>10.45%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.57%</t>
+          <t>-2.71%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>168599</v>
+        <v>88487</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4.51%</t>
+          <t>-3.39%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>93.48%</t>
+          <t>41.03%</t>
         </is>
       </c>
     </row>
@@ -3207,33 +3207,33 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>校园</t>
+          <t>菜场</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>48449</v>
+        <v>48751</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.54%</t>
+          <t>2.36%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3.93%</t>
+          <t>6.07%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>47125</v>
+        <v>28101</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3.95%</t>
+          <t>11.07%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>97.27%</t>
+          <t>57.64%</t>
         </is>
       </c>
     </row>
@@ -3243,33 +3243,33 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>菜场</t>
+          <t>自助</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>42448</v>
+        <v>41468</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2.22%</t>
+          <t>2.01%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-6.76%</t>
+          <t>-21.37%</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>22480</v>
+        <v>15128</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-11.74%</t>
+          <t>23.27%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>52.96%</t>
+          <t>36.48%</t>
         </is>
       </c>
     </row>
@@ -3283,29 +3283,29 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>28048</v>
+        <v>36964</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.47%</t>
+          <t>1.79%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-7.15%</t>
+          <t>-11.13%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>27483</v>
+        <v>35746</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-4.57%</t>
+          <t>-11.76%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>97.99%</t>
+          <t>96.70%</t>
         </is>
       </c>
     </row>
@@ -3315,33 +3315,33 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>自助</t>
+          <t>校园</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>23756</v>
+        <v>20075</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.24%</t>
+          <t>0.97%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6.29%</t>
+          <t>-19.27%</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>10302</v>
+        <v>18985</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-4.80%</t>
+          <t>-20.15%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>43.37%</t>
+          <t>94.57%</t>
         </is>
       </c>
     </row>
@@ -3355,29 +3355,29 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8461</v>
+        <v>7598</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.44%</t>
+          <t>0.37%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-37.80%</t>
+          <t>-34.39%</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>4526</v>
+        <v>4189</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-48.00%</t>
+          <t>-46.91%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>53.49%</t>
+          <t>55.13%</t>
         </is>
       </c>
     </row>
@@ -3391,29 +3391,29 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2924</v>
+        <v>2683</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.15%</t>
+          <t>0.13%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-29.05%</t>
+          <t>-21.46%</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-50.33%</t>
+          <t>-41.58%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>35.57%</t>
+          <t>38.39%</t>
         </is>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -3436,20 +3436,20 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-50.00%</t>
+          <t>3.57%</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>nan%</t>
+          <t>60.00%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>47.37%</t>
+          <t>55.17%</t>
         </is>
       </c>
     </row>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1、当日，山东、上海、四川、福建、辽宁、广东、大连、江苏、山西、浙江地区交易量排名前十。</t>
+          <t>1、当日，福建、上海、四川、山东、辽宁、广东、大连、江苏、浙江、山西地区交易量排名前十。</t>
         </is>
       </c>
     </row>
@@ -3551,33 +3551,33 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>山东</t>
+          <t>福建</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>149411</v>
+        <v>146830</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7.84%</t>
+          <t>7.14%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3.03%</t>
+          <t>3.20%</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>115335</v>
+        <v>85376</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>77.19%</t>
+          <t>58.15%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>3.02%</t>
+          <t>3.13%</t>
         </is>
       </c>
     </row>
@@ -3591,29 +3591,29 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>115565</v>
+        <v>141728</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6.06%</t>
+          <t>6.89%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-6.69%</t>
+          <t>14.40%</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>79302</v>
+        <v>96579</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>68.62%</t>
+          <t>68.14%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>-0.99%</t>
+          <t>13.42%</t>
         </is>
       </c>
     </row>
@@ -3627,29 +3627,29 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>112323</v>
+        <v>126583</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5.89%</t>
+          <t>6.16%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-3.32%</t>
+          <t>-0.74%</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>87316</v>
+        <v>96488</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>77.74%</t>
+          <t>76.23%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>-3.42%</t>
+          <t>1.43%</t>
         </is>
       </c>
     </row>
@@ -3659,33 +3659,33 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>福建</t>
+          <t>山东</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>109095</v>
+        <v>125336</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5.72%</t>
+          <t>6.10%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-4.13%</t>
+          <t>-23.94%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>66062</v>
+        <v>89237</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>60.55%</t>
+          <t>71.20%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>-7.96%</t>
+          <t>-24.00%</t>
         </is>
       </c>
     </row>
@@ -3699,29 +3699,29 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>106034</v>
+        <v>119245</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5.56%</t>
+          <t>5.80%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-21.36%</t>
+          <t>-18.49%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>87532</v>
+        <v>101466</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>82.55%</t>
+          <t>85.09%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>-25.28%</t>
+          <t>-19.92%</t>
         </is>
       </c>
     </row>
@@ -3735,29 +3735,29 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>100829</v>
+        <v>111151</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5.29%</t>
+          <t>5.41%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-9.46%</t>
+          <t>-3.83%</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>43527</v>
+        <v>47339</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>43.17%</t>
+          <t>42.59%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>-13.45%</t>
+          <t>-6.07%</t>
         </is>
       </c>
     </row>
@@ -3771,29 +3771,29 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>95821</v>
+        <v>103778</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5.03%</t>
+          <t>5.05%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3.37%</t>
+          <t>1.33%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>90642</v>
+        <v>96849</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>94.60%</t>
+          <t>93.32%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3.32%</t>
+          <t>0.28%</t>
         </is>
       </c>
     </row>
@@ -3807,29 +3807,29 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>85005</v>
+        <v>83869</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4.46%</t>
+          <t>4.08%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.31%</t>
+          <t>-9.94%</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>53389</v>
+        <v>55939</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>62.81%</t>
+          <t>66.70%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.20%</t>
+          <t>-1.71%</t>
         </is>
       </c>
     </row>
@@ -3839,33 +3839,33 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>山西</t>
+          <t>浙江</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>70619</v>
+        <v>82638</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3.70%</t>
+          <t>4.02%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-0.01%</t>
+          <t>7.10%</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>53989</v>
+        <v>57514</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>76.45%</t>
+          <t>69.60%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1.12%</t>
+          <t>-3.59%</t>
         </is>
       </c>
     </row>
@@ -3875,33 +3875,33 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>浙江</t>
+          <t>山西</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>68177</v>
+        <v>77220</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3.58%</t>
+          <t>3.76%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-3.87%</t>
+          <t>1.02%</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>56083</v>
+        <v>61047</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>82.26%</t>
+          <t>79.06%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>-1.00%</t>
+          <t>10.17%</t>
         </is>
       </c>
     </row>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2、交易笔数TOP10的商户以乘车码交易为主，优惠笔数占比为80.63。</t>
+          <t>2、交易笔数TOP10的商户以乘车码交易为主，优惠笔数占比为83.9。</t>
         </is>
       </c>
     </row>
@@ -4003,33 +4003,33 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>成都红旗连锁股份有限公司</t>
+          <t>上海公交</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>被扫</t>
+          <t>乘车码</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>零售</t>
+          <t>公交地铁</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>22728</v>
+        <v>32946</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-6.64%</t>
+          <t>0.09%</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>21245</v>
+        <v>29352</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>93.48%</t>
+          <t>89.09%</t>
         </is>
       </c>
     </row>
@@ -4039,33 +4039,33 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>上海公交</t>
+          <t>成都红旗连锁股份有限公司</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>乘车码</t>
+          <t>被扫</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>公交地铁</t>
+          <t>零售</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>17646</v>
+        <v>24065</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.42%</t>
+          <t>-3.40%</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>15796</v>
+        <v>22806</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>89.52%</t>
+          <t>94.77%</t>
         </is>
       </c>
     </row>
@@ -4089,19 +4089,19 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>15572</v>
+        <v>20098</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1.31%</t>
+          <t>-3.08%</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>14889</v>
+        <v>19242</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>95.61%</t>
+          <t>95.74%</t>
         </is>
       </c>
     </row>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>昆明日新达商贸有限公司</t>
+          <t>福建省三明市公共交通公司</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -4121,23 +4121,23 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>零售</t>
+          <t>公交地铁</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>15546</v>
+        <v>16393</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2.85%</t>
+          <t>7.91%</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>14682</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>89.56%</t>
         </is>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>上海联华超市发展有限公司</t>
+          <t>昆明日新达商贸有限公司</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -4161,19 +4161,19 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>12064</v>
+        <v>16081</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-18.10%</t>
+          <t>4.97%</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>11511</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>95.42%</t>
+          <t>0.00%</t>
         </is>
       </c>
     </row>
@@ -4183,33 +4183,33 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>工大二食堂猪脚饭</t>
+          <t>青岛公交集团有限责任公司</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>主扫</t>
+          <t>被扫</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>餐饮</t>
+          <t>公交地铁</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>9712</v>
+        <v>13336</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>53.50%</t>
+          <t>1.28%</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>9712</v>
+        <v>12853</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>100.00%</t>
+          <t>96.38%</t>
         </is>
       </c>
     </row>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>永辉超市股份有限公司</t>
+          <t>上海联华超市发展有限公司</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -4233,19 +4233,19 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>9550</v>
+        <v>12543</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-11.81%</t>
+          <t>24.21%</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>6469</v>
+        <v>11957</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>67.74%</t>
+          <t>95.33%</t>
         </is>
       </c>
     </row>
@@ -4255,33 +4255,33 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>工大二食堂烤肉饭</t>
+          <t>滨海公交</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>主扫</t>
+          <t>乘车码</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>餐饮</t>
+          <t>公交地铁</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>9347</v>
+        <v>11925</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>39.67%</t>
+          <t>0.90%</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>9347</v>
+        <v>9760</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>100.00%</t>
+          <t>81.84%</t>
         </is>
       </c>
     </row>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>滨海公交</t>
+          <t>成都地铁</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4305,19 +4305,19 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>9095</v>
+        <v>11332</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>-1.07%</t>
+          <t>1.46%</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>7487</v>
+        <v>10790</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>82.32%</t>
+          <t>95.22%</t>
         </is>
       </c>
     </row>
@@ -4327,33 +4327,33 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>青岛公交集团有限责任公司</t>
+          <t>广州将美信息科技有限公司</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>被扫</t>
+          <t>主扫</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>公交地铁</t>
+          <t>零售</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>8804</v>
+        <v>10682</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1.16%</t>
+          <t>133.49%</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>8418</v>
+        <v>10682</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>95.62%</t>
+          <t>100.00%</t>
         </is>
       </c>
     </row>

</xml_diff>